<commit_message>
Exact ray trace sheet added
A sheet is added including exact ray trace method from "Modern Geometrical Optics" by Richard Ditteon, Wiley Interscience. New York, NY 1998, Chapter 6.  
This traces two a marginal axial ray for an object at infinity. Two ray heights are used. One at the maximum radius of the primary mirror, and one clearing by the secondary mirror by just a bit. These were verified against a manual exact ray trace for the maximum radius, full field marginal axial ray.
</commit_message>
<xml_diff>
--- a/NOFS-Telescopes.xlsx
+++ b/NOFS-Telescopes.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bob.zavala/Desktop/bobMacBackUp/Optics/Ray tracing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A64E115-4D50-B94F-8225-3247066CE234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28B7788-A60D-F646-8829-AFAC01CC2332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="3460" windowWidth="47780" windowHeight="16760" xr2:uid="{9120E6CE-487D-4A4E-A0CB-02EC34448099}"/>
+    <workbookView xWindow="15580" yWindow="1440" windowWidth="44560" windowHeight="25060" activeTab="1" xr2:uid="{9120E6CE-487D-4A4E-A0CB-02EC34448099}"/>
   </bookViews>
   <sheets>
     <sheet name="NOFS" sheetId="2" r:id="rId1"/>
+    <sheet name="Exact trace" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,6 +59,7 @@
     <author>tc={D9869BD4-6229-984D-AA75-E2711985E400}</author>
     <author>tc={7B1F4DCB-9E16-DF4A-AABB-8CB4BFB2BBBF}</author>
     <author>tc={E9CD66AE-FB9F-574A-B74C-C41D982DEA62}</author>
+    <author>tc={671D3686-500B-8C4F-ABC4-908D8B045A47}</author>
   </authors>
   <commentList>
     <comment ref="A5" authorId="0" shapeId="0" xr:uid="{3AAA742A-42EE-1F4C-8616-8A30E5484FAF}">
@@ -220,12 +222,20 @@
     relative secondary magnification from system i-prime and i image distances</t>
       </text>
     </comment>
+    <comment ref="V14" authorId="20" shapeId="0" xr:uid="{671D3686-500B-8C4F-ABC4-908D8B045A47}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is, in terms of system focal length, 0.38 f.l. and larger to the "best astigmatic" median Rm of 0.3 of system f.l. for a classical Cassegrain and R-C which would be a bit less than 0.3 for 1.89 secondary magnification. D-K is slightly more curved. </t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
   <si>
     <t>Diam. (mm)</t>
   </si>
@@ -1864,20 +1874,546 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>Median field curvature R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (mm)</t>
+    </r>
+  </si>
+  <si>
+    <t>Telescope</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>Exact Ray Trace</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Direction cosine check</t>
+  </si>
+  <si>
+    <r>
+      <t>cos(I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <t>Δ</t>
+  </si>
+  <si>
+    <t>γ</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Full Radius Marginal Ray</t>
+  </si>
+  <si>
+    <r>
+      <t>μ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria Math"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <t>to Mirror 1    (0 - 1)</t>
+  </si>
+  <si>
+    <t>to Mirror 2 (1 - 2)</t>
+  </si>
+  <si>
+    <t>to Focal Plane (2 -3)</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <r>
+      <t>T for Y</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.0 (mm)</t>
+    </r>
+  </si>
+  <si>
+    <t>t2 for diffraction focus (mm)</t>
+  </si>
+  <si>
+    <r>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (mm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (mm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (mm)</t>
+    </r>
+  </si>
+  <si>
+    <t>(mm)</t>
+  </si>
+  <si>
+    <t>ξ   (mm)</t>
+  </si>
+  <si>
+    <t>T (mm)</t>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (mm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (mm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (mm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (mm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (mm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Abadi MT Condensed Extra Bold"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (mm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1/mm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1/mm)</t>
+    </r>
+  </si>
+  <si>
+    <t>t1 (mm)</t>
+  </si>
+  <si>
+    <t>t2 (focus) (mm)</t>
+  </si>
+  <si>
+    <t>Min. Radius Marginal Ray</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1914,17 +2450,56 @@
       <name val="Aptos Narrow (Body)"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <vertAlign val="superscript"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Abadi MT Condensed Extra Bold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria Math"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria Math"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1947,7 +2522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1991,6 +2566,27 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2006,6 +2602,140 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>34773</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>14512</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="201084" cy="189604"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4ACDFF9-E7E7-F7C3-C321-6206A2092DD7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="34773" y="3107869"/>
+              <a:ext cx="201084" cy="189604"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1200" b="1" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝝌</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4ACDFF9-E7E7-F7C3-C321-6206A2092DD7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="34773" y="3107869"/>
+              <a:ext cx="201084" cy="189604"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝝌</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2391,6 +3121,9 @@
   <threadedComment ref="G14" dT="2025-12-05T18:56:25.76" personId="{8C851638-141B-034A-B4A3-8E6355A961FE}" id="{E9CD66AE-FB9F-574A-B74C-C41D982DEA62}">
     <text>relative secondary magnification from system i-prime and i image distances</text>
   </threadedComment>
+  <threadedComment ref="V14" dT="2026-01-20T16:35:59.80" personId="{8C851638-141B-034A-B4A3-8E6355A961FE}" id="{671D3686-500B-8C4F-ABC4-908D8B045A47}">
+    <text xml:space="preserve">This is, in terms of system focal length, 0.38 f.l. and larger to the "best astigmatic" median Rm of 0.3 of system f.l. for a classical Cassegrain and R-C which would be a bit less than 0.3 for 1.89 secondary magnification. D-K is slightly more curved. </text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2398,8 +3131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BF685D-8724-5246-AEF2-3915C8A371E5}">
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3027,6 +3760,9 @@
       <c r="U14" s="10" t="s">
         <v>48</v>
       </c>
+      <c r="V14" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="15" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -3103,10 +3839,645 @@
       <c r="U15" s="5">
         <f>R15/32</f>
         <v>59.318375800045942</v>
+      </c>
+      <c r="V15" s="1">
+        <f>-1*((1+I15)*D5*H15^2)/(2*((H15^2-2)*(H15-I15)+(H15+1)*H15-1*(H15^2-1)*(H15-I15)^2/(2*H15)))</f>
+        <v>1073.4672092007195</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3D5ED7-AD07-A046-96A1-F16751D23497}">
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="15" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
+        <v>0</v>
+      </c>
+      <c r="B3" s="15">
+        <v>200</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1500</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15">
+        <v>0</v>
+      </c>
+      <c r="G3" s="15">
+        <v>1</v>
+      </c>
+      <c r="H3" s="11">
+        <f>-3048</f>
+        <v>-3048</v>
+      </c>
+      <c r="I3" s="11">
+        <v>-2865</v>
+      </c>
+      <c r="J3" s="15">
+        <f>1/-3048</f>
+        <v>-3.2808398950131233E-4</v>
+      </c>
+      <c r="K3" s="15">
+        <f>1/-2865</f>
+        <v>-3.4904013961605586E-4</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="5">
+        <v>-885</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="15" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
+        <v>0</v>
+      </c>
+      <c r="B4" s="15">
+        <v>90</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>1500</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+      <c r="F4" s="15">
+        <v>0</v>
+      </c>
+      <c r="G4" s="15">
+        <v>1</v>
+      </c>
+      <c r="H4" s="11">
+        <f>-3048</f>
+        <v>-3048</v>
+      </c>
+      <c r="I4" s="11">
+        <v>-2865</v>
+      </c>
+      <c r="J4" s="15">
+        <f>1/-3048</f>
+        <v>-3.2808398950131233E-4</v>
+      </c>
+      <c r="K4" s="15">
+        <f>1/-2865</f>
+        <v>-3.4904013961605586E-4</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="M4" s="5">
+        <v>-885</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:14" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:14" ht="43" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="19" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="15">
+        <f>(D3-C3)/G3</f>
+        <v>1500</v>
+      </c>
+      <c r="C11" s="15">
+        <f>(M3 - B19)/B25</f>
+        <v>-886.0612289846415</v>
+      </c>
+      <c r="D11" s="15">
+        <f>(N3 - C19)/C25</f>
+        <v>1219.4574232072262</v>
+      </c>
+      <c r="F11" s="15">
+        <f>(D4-C4)/G4</f>
+        <v>1500</v>
+      </c>
+      <c r="G11" s="1">
+        <f>(M4-F19)/F25</f>
+        <v>-885.21456607857363</v>
+      </c>
+      <c r="H11">
+        <f>(N4-G19)/G25</f>
+        <v>1215.8991890419227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="19" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="15">
+        <f xml:space="preserve"> A3+B11*E3</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="15">
+        <f xml:space="preserve"> B17+C11*B23</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="15">
+        <f xml:space="preserve"> C17+D11*C23</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="15">
+        <f>A4+F11*E4</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="15">
+        <f>F17+G11*F23</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="15">
+        <f>G17+H11*G23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="15">
+        <f>B3+B11*F3</f>
+        <v>200</v>
+      </c>
+      <c r="C13" s="15">
+        <f>B18+C11*B24</f>
+        <v>83.969596508964727</v>
+      </c>
+      <c r="D13" s="15">
+        <f>C18+D11*C24</f>
+        <v>-4.9088625286877203</v>
+      </c>
+      <c r="F13" s="15">
+        <f>B4+F11*F4</f>
+        <v>90</v>
+      </c>
+      <c r="G13" s="15">
+        <f>F18+G11*F24</f>
+        <v>37.746343527691124</v>
+      </c>
+      <c r="H13" s="15">
+        <f>G18+H11*G24</f>
+        <v>-2.04937234108138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="19" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="15">
+        <f>G3-(J3)*(B12*E3+B13*F3)</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="15">
+        <f>B25-1*K3*(C12*B23+C13*B24)</f>
+        <v>0.99522687642442142</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="F14" s="15">
+        <f>G4-J4*(F12*E4+F13*F4)</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="15">
+        <f>F25-1*K4*(G12*F23+G13*F24)</f>
+        <v>0.99903395778882309</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="19" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="15">
+        <f>J3*(B12^2+B13^2)</f>
+        <v>-13.123359580052494</v>
+      </c>
+      <c r="C15" s="15">
+        <f>K3*(C12^2+C13^2)</f>
+        <v>-2.4610447252629464</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="F15" s="15">
+        <f>J4*(F12^2+F13^2)</f>
+        <v>-2.6574803149606301</v>
+      </c>
+      <c r="G15" s="15">
+        <f>K4*(G12^2+G13^2)</f>
+        <v>-0.49730766133000692</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="15">
+        <f>B15/(B14+SQRT(B14^2-1*(J3)*B15))</f>
+        <v>-6.5687579693668177</v>
+      </c>
+      <c r="C16" s="15">
+        <f>C15/(C14+SQRT(C14^2-1*(K3)*C15))</f>
+        <v>-1.2366921594365914</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="F16" s="15">
+        <f>F15/(F14+SQRT(F14^2-1*(J4)*F15))</f>
+        <v>-1.3290299082180017</v>
+      </c>
+      <c r="G16" s="15">
+        <f>G15/(G14+SQRT(G14^G172-1*(K4)*G15))</f>
+        <v>-0.24878479547757346</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="15">
+        <f>B12+B16*E3</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="15">
+        <f>C12+C16*B23</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="15">
+        <f>D12</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="15">
+        <f>F12+F16*E4</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f>G12+G16*F23</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <f>H12+H16*G23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="19" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="15">
+        <f>B13+B16*F3</f>
+        <v>200</v>
+      </c>
+      <c r="C18" s="15">
+        <f>C13+C16*B24</f>
+        <v>83.807650713843927</v>
+      </c>
+      <c r="D18" s="15">
+        <f>D13</f>
+        <v>-4.9088625286877203</v>
+      </c>
+      <c r="F18" s="15">
+        <f>F13+F16*F4</f>
+        <v>90</v>
+      </c>
+      <c r="G18" s="1">
+        <f>G13+G16*F24</f>
+        <v>37.731657918420133</v>
+      </c>
+      <c r="H18" s="1">
+        <f>H13+H16*G24</f>
+        <v>-2.04937234108138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="15">
+        <f>B16*G3</f>
+        <v>-6.5687579693668177</v>
+      </c>
+      <c r="C19" s="15">
+        <f>C16*B25</f>
+        <v>-1.2260428445428131</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="F19" s="15">
+        <f>F16*G4</f>
+        <v>-1.3290299082180017</v>
+      </c>
+      <c r="G19" s="1">
+        <f>G16*F25</f>
+        <v>-0.2483509761228207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="19" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="15">
+        <f>SQRT(B14^2 -1*(J3)*B15)</f>
+        <v>0.99784489567934154</v>
+      </c>
+      <c r="C20" s="15">
+        <f>SQRT(C14^2 -1*(K3)*C15)</f>
+        <v>0.99479522122042963</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="F20" s="15">
+        <f>SQRT(F14^2 -1*(J4)*F15)</f>
+        <v>0.99956396656554525</v>
+      </c>
+      <c r="G20" s="1">
+        <f>SQRT(G14^2-1*K4*G15)</f>
+        <v>0.99894707991948062</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="15">
+        <f>2*B20</f>
+        <v>1.9956897913586831</v>
+      </c>
+      <c r="C21" s="15">
+        <f>2*C20</f>
+        <v>1.9895904424408593</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="F21" s="15">
+        <f>2*F20</f>
+        <v>1.9991279331310905</v>
+      </c>
+      <c r="G21" s="15">
+        <f>2*G20</f>
+        <v>1.9978941598389612</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="15">
+        <v>-1</v>
+      </c>
+      <c r="C22" s="15">
+        <v>-1</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="F22" s="15">
+        <v>-1</v>
+      </c>
+      <c r="G22" s="15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="19" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="15">
+        <f>B22*E3-1*B21*J3*B17</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="15">
+        <f>C22*B23-1*C21*K3*C17</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="F23" s="15">
+        <f>F22*E4-1*F21*J4*F17</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="15">
+        <f>G22*F23-1*G21*K4*G17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="15">
+        <f>B22*E3-1*B21*J3*B18</f>
+        <v>0.13095077371119968</v>
+      </c>
+      <c r="C24" s="15">
+        <f>C22*B24-1*C21*K3*C18</f>
+        <v>-7.2750808313752649E-2</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="F24" s="15">
+        <f>F22*F4-1*F21*J4*F18</f>
+        <v>5.9029368104264478E-2</v>
+      </c>
+      <c r="G24" s="15">
+        <f>G22*F24-1*G21*K4*G18</f>
+        <v>-3.2717375435415239E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="15">
+        <f>B22*G3-1*B21*(J3*B19 - 1)</f>
+        <v>0.99138887166663214</v>
+      </c>
+      <c r="C25" s="15">
+        <f>C22*B25-1*C21*(K3*C19 - 1)</f>
+        <v>0.99735014908992503</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="F25" s="15">
+        <f>F22*G3-1*F21*(J4*F19 - 1)</f>
+        <v>0.9982562465124929</v>
+      </c>
+      <c r="G25" s="15">
+        <f>G22*F25-1*G21*(K4*G19 - 1)</f>
+        <v>0.99946472695132504</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="15">
+        <f>B23^2+B24^2+B25^2</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C26" s="15">
+        <f>C23^2+C24^2+C25^2</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="F26" s="15">
+        <f>F23^2+F24^2+F25^2</f>
+        <v>0.99999999999999967</v>
+      </c>
+      <c r="G26" s="15">
+        <f>G23^2+G24^2+G25^2</f>
+        <v>1.0000001670752685</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="1">
+        <f>-1*C18/C24</f>
+        <v>1151.9823993213436</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="1">
+        <f>-1*G18/G24</f>
+        <v>1153.2605356106021</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="15">
+        <f>D27*C25+C19</f>
+        <v>1147.7037748675687</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H28" s="15">
+        <f>H27*G25+G19</f>
+        <v>1152.3948753516665</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>